<commit_message>
regenerated results after fixing tokay fs error
</commit_message>
<xml_diff>
--- a/results/soae/SOAE Results (PW=False, BW=50Hz, rho=1.0, Flattop)/SOAE N_xi Fitted Parameters (PW=False, BW=50Hz, rho=1.0, Flattop).xlsx
+++ b/results/soae/SOAE Results (PW=False, BW=50Hz, rho=1.0, Flattop)/SOAE N_xi Fitted Parameters (PW=False, BW=50Hz, rho=1.0, Flattop).xlsx
@@ -503,7 +503,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -511,44 +511,44 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>tokay_GG1rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1235.467529296875</v>
+        <v>1342.7734375</v>
       </c>
       <c r="E2" t="n">
-        <v>18.30668826242178</v>
+        <v>10.69166059430503</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3690403861639351</v>
+        <v>0.1760964723817636</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01481761991174338</v>
+        <v>0.007962371235322438</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0002987050468043964</v>
+        <v>0.0001311438456137643</v>
       </c>
       <c r="I2" t="n">
-        <v>1.244989836203278</v>
+        <v>0.7695268930878842</v>
       </c>
       <c r="J2" t="n">
-        <v>0.02952978345395024</v>
+        <v>0.0172105369211576</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0002007714665117125</v>
+        <v>1.986000088344137e-05</v>
       </c>
       <c r="L2" t="n">
-        <v>0.03900226757369615</v>
+        <v>0.024</v>
       </c>
       <c r="M2" t="n">
-        <v>48.18603515625</v>
+        <v>32.22656249999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -556,44 +556,44 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>tokay_GG1rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2153.3203125</v>
+        <v>1779.1748046875</v>
       </c>
       <c r="E3" t="n">
-        <v>25.29690995494933</v>
+        <v>17.32916630410013</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5953484429533717</v>
+        <v>0.4232590709113763</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01174786203803543</v>
+        <v>0.009740002083237621</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0002764792769089581</v>
+        <v>0.000237896281914648</v>
       </c>
       <c r="I3" t="n">
-        <v>1.167710898172541</v>
+        <v>0.9570870177067973</v>
       </c>
       <c r="J3" t="n">
-        <v>0.03010231031943876</v>
+        <v>0.03301417938806337</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0002225317243756103</v>
+        <v>7.663130739317239e-05</v>
       </c>
       <c r="L3" t="n">
         <v>0.03</v>
       </c>
       <c r="M3" t="n">
-        <v>64.599609375</v>
+        <v>53.37524414062499</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -601,44 +601,44 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>tokay_GG1rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3703.7109375</v>
+        <v>3649.90234375</v>
       </c>
       <c r="E4" t="n">
-        <v>41.5281063900438</v>
+        <v>33.75892247630429</v>
       </c>
       <c r="F4" t="n">
-        <v>1.08915715665557</v>
+        <v>1.028840650113268</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01121256682576724</v>
+        <v>0.009249267321935947</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0002940718579379065</v>
+        <v>0.0002818816924992607</v>
       </c>
       <c r="I4" t="n">
-        <v>1.144163426792343</v>
+        <v>0.7199080342510847</v>
       </c>
       <c r="J4" t="n">
-        <v>0.02870813548916876</v>
+        <v>0.02708342108361399</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0003427227295027247</v>
+        <v>7.995199215624267e-05</v>
       </c>
       <c r="L4" t="n">
-        <v>0.02700680272108844</v>
+        <v>0.025</v>
       </c>
       <c r="M4" t="n">
-        <v>100.025390625</v>
+        <v>91.24755859375</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -646,44 +646,44 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>tokay_GG1rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4500.439453125</v>
+        <v>4211.425781249999</v>
       </c>
       <c r="E5" t="n">
-        <v>41.23098553500826</v>
+        <v>46.12704065170114</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8730723387695426</v>
+        <v>1.075126454008817</v>
       </c>
       <c r="G5" t="n">
-        <v>0.009161546547721784</v>
+        <v>0.01095283237735466</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0001939971302498696</v>
+        <v>0.0002552879974272531</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8167438705775404</v>
+        <v>1.12866937685471</v>
       </c>
       <c r="J5" t="n">
-        <v>0.02165438031769892</v>
+        <v>0.03671680144623923</v>
       </c>
       <c r="K5" t="n">
-        <v>5.204528376960065e-05</v>
+        <v>0.0001037269999680694</v>
       </c>
       <c r="L5" t="n">
-        <v>0.02600907029478458</v>
+        <v>0.032</v>
       </c>
       <c r="M5" t="n">
-        <v>117.05224609375</v>
+        <v>134.765625</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -691,44 +691,44 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>tokay_GG2rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>966.302490234375</v>
+        <v>1364.1357421875</v>
       </c>
       <c r="E6" t="n">
-        <v>11.16111458848785</v>
+        <v>11.17892505535753</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2845045168068702</v>
+        <v>0.5165510225718823</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01155033201433719</v>
+        <v>0.008194877320222721</v>
       </c>
       <c r="H6" t="n">
-        <v>0.000294425937718389</v>
+        <v>0.0003786654118039249</v>
       </c>
       <c r="I6" t="n">
-        <v>1.03959466091058</v>
+        <v>0.6745621062333408</v>
       </c>
       <c r="J6" t="n">
-        <v>0.03580911673450345</v>
+        <v>0.04402790446511812</v>
       </c>
       <c r="K6" t="n">
-        <v>0.000121007859575912</v>
+        <v>7.726461382615047e-05</v>
       </c>
       <c r="L6" t="n">
-        <v>0.03299319727891156</v>
+        <v>0.022</v>
       </c>
       <c r="M6" t="n">
-        <v>31.88140869140625</v>
+        <v>30.01098632812499</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -736,44 +736,44 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>tokay_GG2rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3022.723388671875</v>
+        <v>1776.123046875</v>
       </c>
       <c r="E7" t="n">
-        <v>32.85410002839859</v>
+        <v>15.89647682661615</v>
       </c>
       <c r="F7" t="n">
-        <v>0.991437602134656</v>
+        <v>0.7054151176192633</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0108690395394843</v>
+        <v>0.008950098842861824</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0003279948161483192</v>
+        <v>0.0003971656799681791</v>
       </c>
       <c r="I7" t="n">
-        <v>1.062929278007326</v>
+        <v>0.7173081035430412</v>
       </c>
       <c r="J7" t="n">
-        <v>0.05328801022286783</v>
+        <v>0.04246533504862162</v>
       </c>
       <c r="K7" t="n">
-        <v>8.314328915240177e-05</v>
+        <v>0.0001014996746024675</v>
       </c>
       <c r="L7" t="n">
-        <v>0.03399092970521542</v>
+        <v>0.023</v>
       </c>
       <c r="M7" t="n">
-        <v>102.7451782226562</v>
+        <v>40.85083007812499</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -781,44 +781,44 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>tokay_GG2rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3151.922607421875</v>
+        <v>3607.177734375</v>
       </c>
       <c r="E8" t="n">
-        <v>30.40989913739679</v>
+        <v>37.73114265379662</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8302988362606313</v>
+        <v>1.449612615928588</v>
       </c>
       <c r="G8" t="n">
-        <v>0.009648047533207253</v>
+        <v>0.01046001761827079</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0002634261495842301</v>
+        <v>0.0004018689187711335</v>
       </c>
       <c r="I8" t="n">
-        <v>1.094492102218201</v>
+        <v>0.9157383972568074</v>
       </c>
       <c r="J8" t="n">
-        <v>0.03294355000433496</v>
+        <v>0.03712832976532102</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0001923642166464746</v>
+        <v>0.0003092315633094102</v>
       </c>
       <c r="L8" t="n">
-        <v>0.02399092970521542</v>
+        <v>0.025</v>
       </c>
       <c r="M8" t="n">
-        <v>75.6175537109375</v>
+        <v>90.179443359375</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -826,44 +826,44 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>tokay_GG2rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>3954.034423828125</v>
+        <v>4394.531249999999</v>
       </c>
       <c r="E9" t="n">
-        <v>31.86512210603134</v>
+        <v>40.65544364344527</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5955162417458386</v>
+        <v>1.63784606723683</v>
       </c>
       <c r="G9" t="n">
-        <v>0.008058888388528725</v>
+        <v>0.00925137206464177</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0001506097767275596</v>
+        <v>0.0003727009717445588</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8485684437948837</v>
+        <v>0.6583620360973251</v>
       </c>
       <c r="J9" t="n">
-        <v>0.01568742471093194</v>
+        <v>0.0297556066450585</v>
       </c>
       <c r="K9" t="n">
-        <v>6.257251609513855e-05</v>
+        <v>0.0001351758422769943</v>
       </c>
       <c r="L9" t="n">
-        <v>0.02</v>
+        <v>0.023</v>
       </c>
       <c r="M9" t="n">
-        <v>79.0806884765625</v>
+        <v>101.07421875</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -871,44 +871,44 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>tokay_GG3rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1811.480712890625</v>
+        <v>1257.32421875</v>
       </c>
       <c r="E10" t="n">
-        <v>23.97310956875118</v>
+        <v>14.32494353004988</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2823202957666863</v>
+        <v>0.5390601189704403</v>
       </c>
       <c r="G10" t="n">
-        <v>0.01323398554461929</v>
+        <v>0.01139319780564744</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0001558505667533058</v>
+        <v>0.0004287359703500823</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8390822319957771</v>
+        <v>0.8770891908533835</v>
       </c>
       <c r="J10" t="n">
-        <v>0.01603815453141878</v>
+        <v>0.04174508411430886</v>
       </c>
       <c r="K10" t="n">
-        <v>1.20314767802092e-05</v>
+        <v>0.0001964491379633126</v>
       </c>
       <c r="L10" t="n">
-        <v>0.04299319727891156</v>
+        <v>0.03</v>
       </c>
       <c r="M10" t="n">
-        <v>77.88134765625</v>
+        <v>37.71972656249999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -916,44 +916,44 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>tokay_GG3rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2177.545166015625</v>
+        <v>1837.158203125</v>
       </c>
       <c r="E11" t="n">
-        <v>28.52641489875884</v>
+        <v>13.69192523662817</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8644506715203875</v>
+        <v>0.6034139080106731</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0131002632431984</v>
+        <v>0.007452774188601861</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0003969840373516205</v>
+        <v>0.0003284496169052116</v>
       </c>
       <c r="I11" t="n">
-        <v>1.259398907356392</v>
+        <v>0.706938380258768</v>
       </c>
       <c r="J11" t="n">
-        <v>0.03694001935170459</v>
+        <v>0.04688690934595412</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0006131002388727199</v>
+        <v>5.914898884343351e-05</v>
       </c>
       <c r="L11" t="n">
-        <v>0.03099773242630385</v>
+        <v>0.021</v>
       </c>
       <c r="M11" t="n">
-        <v>67.49896240234375</v>
+        <v>38.580322265625</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -961,44 +961,44 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>tokay_GG3rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3111.5478515625</v>
+        <v>2578.7353515625</v>
       </c>
       <c r="E12" t="n">
-        <v>29.68215229911629</v>
+        <v>18.99626220687842</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4267803169559746</v>
+        <v>0.6072719896218819</v>
       </c>
       <c r="G12" t="n">
-        <v>0.009539352667904833</v>
+        <v>0.007366503195207008</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0001371601329356584</v>
+        <v>0.0002354921722595246</v>
       </c>
       <c r="I12" t="n">
-        <v>1.056193478412823</v>
+        <v>0.8303156667294969</v>
       </c>
       <c r="J12" t="n">
-        <v>0.01554751289709087</v>
+        <v>0.04097745306654904</v>
       </c>
       <c r="K12" t="n">
-        <v>6.473141480524591e-05</v>
+        <v>5.044628888431499e-05</v>
       </c>
       <c r="L12" t="n">
-        <v>0.02399092970521542</v>
+        <v>0.023</v>
       </c>
       <c r="M12" t="n">
-        <v>74.64892578125</v>
+        <v>59.31091308593749</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1006,44 +1006,44 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>tokay_GG3rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3477.6123046875</v>
+        <v>3567.5048828125</v>
       </c>
       <c r="E13" t="n">
-        <v>31.06055555179859</v>
+        <v>34.97447838578351</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9146717045149659</v>
+        <v>1.249344345561586</v>
       </c>
       <c r="G13" t="n">
-        <v>0.008931575124096447</v>
+        <v>0.009803624531611243</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0002630171578591648</v>
+        <v>0.0003502011592417628</v>
       </c>
       <c r="I13" t="n">
-        <v>1.116934099595815</v>
+        <v>0.8817297569450167</v>
       </c>
       <c r="J13" t="n">
-        <v>0.03814322740928681</v>
+        <v>0.03434207674933716</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0002135071431182884</v>
+        <v>0.0002175897622740973</v>
       </c>
       <c r="L13" t="n">
-        <v>0.02399092970521542</v>
+        <v>0.024</v>
       </c>
       <c r="M13" t="n">
-        <v>83.43115234375</v>
+        <v>85.62011718749999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1051,44 +1051,44 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ACsb30learSOAEwfA2.mat</t>
+          <t>tokay_GG4rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1798.0224609375</v>
+        <v>1251.220703125</v>
       </c>
       <c r="E14" t="n">
-        <v>19.97564891497187</v>
+        <v>13.65795908537932</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6034139717733831</v>
+        <v>0.5145027674971088</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01110978830851559</v>
+        <v>0.0109157073977978</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0003355986840446694</v>
+        <v>0.0004112006508620796</v>
       </c>
       <c r="I14" t="n">
-        <v>0.974712081647007</v>
+        <v>1.002510682548067</v>
       </c>
       <c r="J14" t="n">
-        <v>0.03018685437935022</v>
+        <v>0.04889588957124038</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0002432732121475753</v>
+        <v>0.0002279447290236955</v>
       </c>
       <c r="L14" t="n">
-        <v>0.02600907029478458</v>
+        <v>0.029</v>
       </c>
       <c r="M14" t="n">
-        <v>46.764892578125</v>
+        <v>36.28540039062499</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1096,44 +1096,44 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ACsb30learSOAEwfA2.mat</t>
+          <t>tokay_GG4rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2139.862060546875</v>
+        <v>2590.9423828125</v>
       </c>
       <c r="E15" t="n">
-        <v>16.10257133355928</v>
+        <v>24.41431871821503</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4154622733024121</v>
+        <v>0.8301093520243699</v>
       </c>
       <c r="G15" t="n">
-        <v>0.007525051091117537</v>
+        <v>0.009422949302219909</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0001941537639095458</v>
+        <v>0.0003203889663973446</v>
       </c>
       <c r="I15" t="n">
-        <v>0.7013784437903158</v>
+        <v>0.8328716851602599</v>
       </c>
       <c r="J15" t="n">
-        <v>0.02065205830061842</v>
+        <v>0.03451331485304102</v>
       </c>
       <c r="K15" t="n">
-        <v>5.43952414301807e-05</v>
+        <v>0.0001365347929539875</v>
       </c>
       <c r="L15" t="n">
-        <v>0.02</v>
+        <v>0.025</v>
       </c>
       <c r="M15" t="n">
-        <v>42.7972412109375</v>
+        <v>64.77355957031249</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1141,44 +1141,44 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ACsb30learSOAEwfA2.mat</t>
+          <t>tokay_GG4rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2417.10205078125</v>
+        <v>3216.552734375</v>
       </c>
       <c r="E16" t="n">
-        <v>20.27253682937761</v>
+        <v>29.62648422299942</v>
       </c>
       <c r="F16" t="n">
-        <v>0.5366492113889888</v>
+        <v>1.131505733697491</v>
       </c>
       <c r="G16" t="n">
-        <v>0.008387124913830249</v>
+        <v>0.009210632210808778</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0002220217434408838</v>
+        <v>0.0003517759002068254</v>
       </c>
       <c r="I16" t="n">
-        <v>0.5896820563668638</v>
+        <v>0.6740010612060136</v>
       </c>
       <c r="J16" t="n">
-        <v>0.01678981563699513</v>
+        <v>0.03159363569920032</v>
       </c>
       <c r="K16" t="n">
-        <v>4.925455955194371e-05</v>
+        <v>0.0001020011721056376</v>
       </c>
       <c r="L16" t="n">
-        <v>0.02099773242630385</v>
+        <v>0.024</v>
       </c>
       <c r="M16" t="n">
-        <v>50.753662109375</v>
+        <v>77.19726562499999</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1186,44 +1186,44 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ACsb30learSOAEwfA2.mat</t>
+          <t>tokay_GG4rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2783.16650390625</v>
+        <v>3582.763671875</v>
       </c>
       <c r="E17" t="n">
-        <v>25.43828047953511</v>
+        <v>34.52374034953</v>
       </c>
       <c r="F17" t="n">
-        <v>1.144779192487545</v>
+        <v>1.415655296318656</v>
       </c>
       <c r="G17" t="n">
-        <v>0.009140049811548031</v>
+        <v>0.009636064086655871</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0004113225676152744</v>
+        <v>0.0003951294101343249</v>
       </c>
       <c r="I17" t="n">
-        <v>0.5115609906061731</v>
+        <v>0.7348881400323389</v>
       </c>
       <c r="J17" t="n">
-        <v>0.02370136063912024</v>
+        <v>0.02998586396090274</v>
       </c>
       <c r="K17" t="n">
-        <v>0.000125193771606749</v>
+        <v>0.0002236340154518327</v>
       </c>
       <c r="L17" t="n">
-        <v>0.02199546485260771</v>
+        <v>0.022</v>
       </c>
       <c r="M17" t="n">
-        <v>61.217041015625</v>
+        <v>78.82080078124999</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1231,44 +1231,44 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4350.5859375</v>
+        <v>1235.467529296875</v>
       </c>
       <c r="E18" t="n">
-        <v>38.18817150603999</v>
+        <v>18.30668826242178</v>
       </c>
       <c r="F18" t="n">
-        <v>2.062741876737991</v>
+        <v>0.3690403861639351</v>
       </c>
       <c r="G18" t="n">
-        <v>0.008777707659300775</v>
+        <v>0.01481761991174338</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0004741296704331543</v>
+        <v>0.0002987050468043964</v>
       </c>
       <c r="I18" t="n">
-        <v>0.4666897477044611</v>
+        <v>1.244989836203278</v>
       </c>
       <c r="J18" t="n">
-        <v>0.02632494419016262</v>
+        <v>0.02952978345395024</v>
       </c>
       <c r="K18" t="n">
-        <v>0.0001339445586304853</v>
+        <v>0.0002007714665117125</v>
       </c>
       <c r="L18" t="n">
-        <v>0.021</v>
+        <v>0.03900226757369615</v>
       </c>
       <c r="M18" t="n">
-        <v>91.3623046875</v>
+        <v>48.18603515625</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1276,44 +1276,44 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7453.125</v>
+        <v>2153.3203125</v>
       </c>
       <c r="E19" t="n">
-        <v>69.19801128502411</v>
+        <v>25.29690995494933</v>
       </c>
       <c r="F19" t="n">
-        <v>1.29562100210892</v>
+        <v>0.5953484429533717</v>
       </c>
       <c r="G19" t="n">
-        <v>0.009284429187089188</v>
+        <v>0.01174786203803543</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0001738359415827481</v>
+        <v>0.0002764792769089581</v>
       </c>
       <c r="I19" t="n">
-        <v>0.5678163655099446</v>
+        <v>1.167710898172541</v>
       </c>
       <c r="J19" t="n">
-        <v>0.01095659896956142</v>
+        <v>0.03010231031943876</v>
       </c>
       <c r="K19" t="n">
-        <v>2.903193464227278e-05</v>
+        <v>0.0002225317243756103</v>
       </c>
       <c r="L19" t="n">
-        <v>0.023</v>
+        <v>0.03</v>
       </c>
       <c r="M19" t="n">
-        <v>171.421875</v>
+        <v>64.599609375</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1321,44 +1321,44 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>8452.1484375</v>
+        <v>3703.7109375</v>
       </c>
       <c r="E20" t="n">
-        <v>69.4790088667789</v>
+        <v>41.5281063900438</v>
       </c>
       <c r="F20" t="n">
-        <v>1.153285808860182</v>
+        <v>1.08915715665557</v>
       </c>
       <c r="G20" t="n">
-        <v>0.008220277883256105</v>
+        <v>0.01121256682576724</v>
       </c>
       <c r="H20" t="n">
-        <v>0.000136448835155728</v>
+        <v>0.0002940718579379065</v>
       </c>
       <c r="I20" t="n">
-        <v>0.6154222216427551</v>
+        <v>1.144163426792343</v>
       </c>
       <c r="J20" t="n">
-        <v>0.008877207013722566</v>
+        <v>0.02870813548916876</v>
       </c>
       <c r="K20" t="n">
-        <v>3.359224672051262e-05</v>
+        <v>0.0003427227295027247</v>
       </c>
       <c r="L20" t="n">
-        <v>0.019</v>
+        <v>0.02700680272108844</v>
       </c>
       <c r="M20" t="n">
-        <v>160.5908203125</v>
+        <v>100.025390625</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1366,44 +1366,44 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>9026.3671875</v>
+        <v>4500.439453125</v>
       </c>
       <c r="E21" t="n">
-        <v>81.38665497811712</v>
+        <v>41.23098553500826</v>
       </c>
       <c r="F21" t="n">
-        <v>2.179639449356527</v>
+        <v>0.8730723387695426</v>
       </c>
       <c r="G21" t="n">
-        <v>0.00901654600211965</v>
+        <v>0.009161546547721784</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0002414747155838022</v>
+        <v>0.0001939971302498696</v>
       </c>
       <c r="I21" t="n">
-        <v>0.721227100608454</v>
+        <v>0.8167438705775404</v>
       </c>
       <c r="J21" t="n">
-        <v>0.01785733306857111</v>
+        <v>0.02165438031769892</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0001004126253638873</v>
+        <v>5.204528376960065e-05</v>
       </c>
       <c r="L21" t="n">
-        <v>0.02</v>
+        <v>0.02600907029478458</v>
       </c>
       <c r="M21" t="n">
-        <v>180.52734375</v>
+        <v>117.05224609375</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1411,44 +1411,44 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>6837.890625</v>
+        <v>966.302490234375</v>
       </c>
       <c r="E22" t="n">
-        <v>61.14423462696202</v>
+        <v>11.16111458848785</v>
       </c>
       <c r="F22" t="n">
-        <v>2.43283311556865</v>
+        <v>0.2845045168068702</v>
       </c>
       <c r="G22" t="n">
-        <v>0.008941973187376337</v>
+        <v>0.01155033201433719</v>
       </c>
       <c r="H22" t="n">
-        <v>0.000355787076598443</v>
+        <v>0.000294425937718389</v>
       </c>
       <c r="I22" t="n">
-        <v>0.5542966708632717</v>
+        <v>1.03959466091058</v>
       </c>
       <c r="J22" t="n">
-        <v>0.02302424109636626</v>
+        <v>0.03580911673450345</v>
       </c>
       <c r="K22" t="n">
-        <v>0.0001126053621516931</v>
+        <v>0.000121007859575912</v>
       </c>
       <c r="L22" t="n">
-        <v>0.022</v>
+        <v>0.03299319727891156</v>
       </c>
       <c r="M22" t="n">
-        <v>150.43359375</v>
+        <v>31.88140869140625</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1456,44 +1456,44 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>7901.3671875</v>
+        <v>3022.723388671875</v>
       </c>
       <c r="E23" t="n">
-        <v>72.61693277193591</v>
+        <v>32.85410002839859</v>
       </c>
       <c r="F23" t="n">
-        <v>2.621698804344461</v>
+        <v>0.991437602134656</v>
       </c>
       <c r="G23" t="n">
-        <v>0.009190426295694274</v>
+        <v>0.0108690395394843</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0003318031857185426</v>
+        <v>0.0003279948161483192</v>
       </c>
       <c r="I23" t="n">
-        <v>0.7176820945998618</v>
+        <v>1.062929278007326</v>
       </c>
       <c r="J23" t="n">
-        <v>0.02887872450328945</v>
+        <v>0.05328801022286783</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0001181910140158244</v>
+        <v>8.314328915240177e-05</v>
       </c>
       <c r="L23" t="n">
-        <v>0.022</v>
+        <v>0.03399092970521542</v>
       </c>
       <c r="M23" t="n">
-        <v>173.830078125</v>
+        <v>102.7451782226562</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1501,44 +1501,44 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>8835.9375</v>
+        <v>3151.922607421875</v>
       </c>
       <c r="E24" t="n">
-        <v>75.33983965195233</v>
+        <v>30.40989913739679</v>
       </c>
       <c r="F24" t="n">
-        <v>2.557140366460105</v>
+        <v>0.8302988362606313</v>
       </c>
       <c r="G24" t="n">
-        <v>0.008526524735145799</v>
+        <v>0.009648047533207253</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0002894022695905335</v>
+        <v>0.0002634261495842301</v>
       </c>
       <c r="I24" t="n">
-        <v>0.7128489007584123</v>
+        <v>1.094492102218201</v>
       </c>
       <c r="J24" t="n">
-        <v>0.02314669123347024</v>
+        <v>0.03294355000433496</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0001519252691792823</v>
+        <v>0.0001923642166464746</v>
       </c>
       <c r="L24" t="n">
-        <v>0.02</v>
+        <v>0.02399092970521542</v>
       </c>
       <c r="M24" t="n">
-        <v>176.71875</v>
+        <v>75.6175537109375</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1546,44 +1546,44 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>9257.8125</v>
+        <v>3954.034423828125</v>
       </c>
       <c r="E25" t="n">
-        <v>89.1534077998639</v>
+        <v>31.86512210603134</v>
       </c>
       <c r="F25" t="n">
-        <v>3.259690495762425</v>
+        <v>0.5955162417458386</v>
       </c>
       <c r="G25" t="n">
-        <v>0.009630072741251121</v>
+        <v>0.008058888388528725</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0003521015894156881</v>
+        <v>0.0001506097767275596</v>
       </c>
       <c r="I25" t="n">
-        <v>0.3687694104084971</v>
+        <v>0.8485684437948837</v>
       </c>
       <c r="J25" t="n">
-        <v>0.01107179803851206</v>
+        <v>0.01568742471093194</v>
       </c>
       <c r="K25" t="n">
-        <v>7.302487491588827e-05</v>
+        <v>6.257251609513855e-05</v>
       </c>
       <c r="L25" t="n">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="M25" t="n">
-        <v>194.4140625</v>
+        <v>79.0806884765625</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1591,44 +1591,44 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5625.54931640625</v>
+        <v>1811.480712890625</v>
       </c>
       <c r="E26" t="n">
-        <v>51.83701769448351</v>
+        <v>23.97310956875118</v>
       </c>
       <c r="F26" t="n">
-        <v>2.526739557456056</v>
+        <v>0.2823202957666863</v>
       </c>
       <c r="G26" t="n">
-        <v>0.009214569952005749</v>
+        <v>0.01323398554461929</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0004491542808250064</v>
+        <v>0.0001558505667533058</v>
       </c>
       <c r="I26" t="n">
-        <v>0.7835877415703257</v>
+        <v>0.8390822319957771</v>
       </c>
       <c r="J26" t="n">
-        <v>0.04687451605713499</v>
+        <v>0.01603815453141878</v>
       </c>
       <c r="K26" t="n">
-        <v>0.0002243659335072323</v>
+        <v>1.20314767802092e-05</v>
       </c>
       <c r="L26" t="n">
-        <v>0.02399092970521542</v>
+        <v>0.04299319727891156</v>
       </c>
       <c r="M26" t="n">
-        <v>134.962158203125</v>
+        <v>77.88134765625</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1636,44 +1636,44 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>8096.484375</v>
+        <v>2177.545166015625</v>
       </c>
       <c r="E27" t="n">
-        <v>78.28887462547326</v>
+        <v>28.52641489875884</v>
       </c>
       <c r="F27" t="n">
-        <v>2.624205836221664</v>
+        <v>0.8644506715203875</v>
       </c>
       <c r="G27" t="n">
-        <v>0.009669489990891665</v>
+        <v>0.0131002632431984</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0003241167048163005</v>
+        <v>0.0003969840373516205</v>
       </c>
       <c r="I27" t="n">
-        <v>0.606666242649432</v>
+        <v>1.259398907356392</v>
       </c>
       <c r="J27" t="n">
-        <v>0.02019008849351071</v>
+        <v>0.03694001935170459</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0001021461108885125</v>
+        <v>0.0006131002388727199</v>
       </c>
       <c r="L27" t="n">
-        <v>0.02199546485260771</v>
+        <v>0.03099773242630385</v>
       </c>
       <c r="M27" t="n">
-        <v>178.0859375</v>
+        <v>67.49896240234375</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1681,44 +1681,44 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>8489.46533203125</v>
+        <v>3111.5478515625</v>
       </c>
       <c r="E28" t="n">
-        <v>101.9184343584824</v>
+        <v>29.68215229911629</v>
       </c>
       <c r="F28" t="n">
-        <v>3.481792421635467</v>
+        <v>0.4267803169559746</v>
       </c>
       <c r="G28" t="n">
-        <v>0.01200528306228405</v>
+        <v>0.009539352667904833</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0004101309429344697</v>
+        <v>0.0001371601329356584</v>
       </c>
       <c r="I28" t="n">
-        <v>0.941342888221613</v>
+        <v>1.056193478412823</v>
       </c>
       <c r="J28" t="n">
-        <v>0.03199093798015184</v>
+        <v>0.01554751289709087</v>
       </c>
       <c r="K28" t="n">
-        <v>0.0003485549518335093</v>
+        <v>6.473141480524591e-05</v>
       </c>
       <c r="L28" t="n">
-        <v>0.02800453514739229</v>
+        <v>0.02399092970521542</v>
       </c>
       <c r="M28" t="n">
-        <v>237.7435302734375</v>
+        <v>74.64892578125</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1726,44 +1726,44 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>9864.898681640625</v>
+        <v>3477.6123046875</v>
       </c>
       <c r="E29" t="n">
-        <v>92.57374287449112</v>
+        <v>31.06055555179859</v>
       </c>
       <c r="F29" t="n">
-        <v>3.26948592510969</v>
+        <v>0.9146717045149659</v>
       </c>
       <c r="G29" t="n">
-        <v>0.009384155464949513</v>
+        <v>0.008931575124096447</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0003314262042239185</v>
+        <v>0.0002630171578591648</v>
       </c>
       <c r="I29" t="n">
-        <v>0.6031090155337008</v>
+        <v>1.116934099595815</v>
       </c>
       <c r="J29" t="n">
-        <v>0.02156217105194045</v>
+        <v>0.03814322740928681</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0001095498729547878</v>
+        <v>0.0002135071431182884</v>
       </c>
       <c r="L29" t="n">
-        <v>0.02199546485260771</v>
+        <v>0.02399092970521542</v>
       </c>
       <c r="M29" t="n">
-        <v>216.9830322265625</v>
+        <v>83.43115234375</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1771,44 +1771,44 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>owl_TAG4learSOAEwf1.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>4944.561767578125</v>
+        <v>1798.0224609375</v>
       </c>
       <c r="E30" t="n">
-        <v>45.28841458447616</v>
+        <v>19.97564891497187</v>
       </c>
       <c r="F30" t="n">
-        <v>1.798293050157823</v>
+        <v>0.6034139717733831</v>
       </c>
       <c r="G30" t="n">
-        <v>0.009159237302168175</v>
+        <v>0.01110978830851559</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0003636910882475713</v>
+        <v>0.0003355986840446694</v>
       </c>
       <c r="I30" t="n">
-        <v>0.5391445149782679</v>
+        <v>0.974712081647007</v>
       </c>
       <c r="J30" t="n">
-        <v>0.02201095677423928</v>
+        <v>0.03018685437935022</v>
       </c>
       <c r="K30" t="n">
-        <v>0.0001084582128997591</v>
+        <v>0.0002432732121475753</v>
       </c>
       <c r="L30" t="n">
-        <v>0.02199546485260771</v>
+        <v>0.02600907029478458</v>
       </c>
       <c r="M30" t="n">
-        <v>108.7579345703125</v>
+        <v>46.764892578125</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1816,44 +1816,44 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>owl_TAG4learSOAEwf1.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>5768.206787109375</v>
+        <v>2139.862060546875</v>
       </c>
       <c r="E31" t="n">
-        <v>68.8618131122638</v>
+        <v>16.10257133355928</v>
       </c>
       <c r="F31" t="n">
-        <v>2.105416667748536</v>
+        <v>0.4154622733024121</v>
       </c>
       <c r="G31" t="n">
-        <v>0.01193816651409832</v>
+        <v>0.007525051091117537</v>
       </c>
       <c r="H31" t="n">
-        <v>0.0003650036736639992</v>
+        <v>0.0001941537639095458</v>
       </c>
       <c r="I31" t="n">
-        <v>0.9243709592246925</v>
+        <v>0.7013784437903158</v>
       </c>
       <c r="J31" t="n">
-        <v>0.03284198698865044</v>
+        <v>0.02065205830061842</v>
       </c>
       <c r="K31" t="n">
-        <v>0.0002025271991541933</v>
+        <v>5.43952414301807e-05</v>
       </c>
       <c r="L31" t="n">
-        <v>0.03099773242630385</v>
+        <v>0.02</v>
       </c>
       <c r="M31" t="n">
-        <v>178.8013305664062</v>
+        <v>42.7972412109375</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1861,44 +1861,44 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>owl_TAG4learSOAEwf1.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>7184.014892578125</v>
+        <v>2417.10205078125</v>
       </c>
       <c r="E32" t="n">
-        <v>215.212239384061</v>
+        <v>20.27253682937761</v>
       </c>
       <c r="F32" t="n">
-        <v>3.426336935219513</v>
+        <v>0.5366492113889888</v>
       </c>
       <c r="G32" t="n">
-        <v>0.02995709816893599</v>
+        <v>0.008387124913830249</v>
       </c>
       <c r="H32" t="n">
-        <v>0.0004769390078463361</v>
+        <v>0.0002220217434408838</v>
       </c>
       <c r="I32" t="n">
-        <v>1.272598354498129</v>
+        <v>0.5896820563668638</v>
       </c>
       <c r="J32" t="n">
-        <v>0.01906358170377451</v>
+        <v>0.01678981563699513</v>
       </c>
       <c r="K32" t="n">
-        <v>0.0004631125362880487</v>
+        <v>4.925455955194371e-05</v>
       </c>
       <c r="L32" t="n">
-        <v>0.07099773242630386</v>
+        <v>0.02099773242630385</v>
       </c>
       <c r="M32" t="n">
-        <v>510.0487670898438</v>
+        <v>50.753662109375</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1906,44 +1906,44 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>owl_TAG4learSOAEwf1.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>9633.416748046875</v>
+        <v>2783.16650390625</v>
       </c>
       <c r="E33" t="n">
-        <v>163.3124452650469</v>
+        <v>25.43828047953511</v>
       </c>
       <c r="F33" t="n">
-        <v>3.053847747422519</v>
+        <v>1.144779192487545</v>
       </c>
       <c r="G33" t="n">
-        <v>0.01695270219656568</v>
+        <v>0.009140049811548031</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0003170056717458705</v>
+        <v>0.0004113225676152744</v>
       </c>
       <c r="I33" t="n">
-        <v>1.103992840979661</v>
+        <v>0.5115609906061731</v>
       </c>
       <c r="J33" t="n">
-        <v>0.01949410344315334</v>
+        <v>0.02370136063912024</v>
       </c>
       <c r="K33" t="n">
-        <v>0.0002697444831906281</v>
+        <v>0.000125193771606749</v>
       </c>
       <c r="L33" t="n">
-        <v>0.04099773242630386</v>
+        <v>0.02199546485260771</v>
       </c>
       <c r="M33" t="n">
-        <v>394.9482421875</v>
+        <v>61.217041015625</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1951,44 +1951,44 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>tokay_GG1rearSOAEwf.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1184.326171875</v>
+        <v>4350.5859375</v>
       </c>
       <c r="E34" t="n">
-        <v>9.310205854454773</v>
+        <v>38.18817150603999</v>
       </c>
       <c r="F34" t="n">
-        <v>0.2903424537229921</v>
+        <v>2.062741876737991</v>
       </c>
       <c r="G34" t="n">
-        <v>0.007861183916686611</v>
+        <v>0.008777707659300775</v>
       </c>
       <c r="H34" t="n">
-        <v>0.000245154131199624</v>
+        <v>0.0004741296704331543</v>
       </c>
       <c r="I34" t="n">
-        <v>0.8640555336161992</v>
+        <v>0.4666897477044611</v>
       </c>
       <c r="J34" t="n">
-        <v>0.03993360836185646</v>
+        <v>0.02632494419016262</v>
       </c>
       <c r="K34" t="n">
-        <v>6.366882857903645e-05</v>
+        <v>0.0001339445586304853</v>
       </c>
       <c r="L34" t="n">
-        <v>0.02399092970521542</v>
+        <v>0.021</v>
       </c>
       <c r="M34" t="n">
-        <v>28.4130859375</v>
+        <v>91.3623046875</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1996,44 +1996,44 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>tokay_GG1rearSOAEwf.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1569.232177734375</v>
+        <v>7453.125</v>
       </c>
       <c r="E35" t="n">
-        <v>14.81436467459153</v>
+        <v>69.19801128502411</v>
       </c>
       <c r="F35" t="n">
-        <v>0.4350133700630791</v>
+        <v>1.29562100210892</v>
       </c>
       <c r="G35" t="n">
-        <v>0.00944051803473735</v>
+        <v>0.009284429187089188</v>
       </c>
       <c r="H35" t="n">
-        <v>0.0002772141536704546</v>
+        <v>0.0001738359415827481</v>
       </c>
       <c r="I35" t="n">
-        <v>1.099380851528698</v>
+        <v>0.5678163655099446</v>
       </c>
       <c r="J35" t="n">
-        <v>0.04937351279295597</v>
+        <v>0.01095659896956142</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0001004454495142006</v>
+        <v>2.903193464227278e-05</v>
       </c>
       <c r="L35" t="n">
-        <v>0.02900226757369614</v>
+        <v>0.023</v>
       </c>
       <c r="M35" t="n">
-        <v>45.51129150390625</v>
+        <v>171.421875</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -2041,44 +2041,44 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>tokay_GG1rearSOAEwf.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3216.522216796875</v>
+        <v>8452.1484375</v>
       </c>
       <c r="E36" t="n">
-        <v>31.08714473089632</v>
+        <v>69.4790088667789</v>
       </c>
       <c r="F36" t="n">
-        <v>0.8712655418719807</v>
+        <v>1.153285808860182</v>
       </c>
       <c r="G36" t="n">
-        <v>0.009664831341303149</v>
+        <v>0.008220277883256105</v>
       </c>
       <c r="H36" t="n">
-        <v>0.000270871917912514</v>
+        <v>0.000136448835155728</v>
       </c>
       <c r="I36" t="n">
-        <v>0.7348792527231891</v>
+        <v>0.6154222216427551</v>
       </c>
       <c r="J36" t="n">
-        <v>0.02487920380584942</v>
+        <v>0.008877207013722566</v>
       </c>
       <c r="K36" t="n">
-        <v>7.952559979549744e-05</v>
+        <v>3.359224672051262e-05</v>
       </c>
       <c r="L36" t="n">
-        <v>0.02600907029478458</v>
+        <v>0.019</v>
       </c>
       <c r="M36" t="n">
-        <v>83.65875244140625</v>
+        <v>160.5908203125</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -2086,44 +2086,44 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>tokay_GG1rearSOAEwf.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>3714.4775390625</v>
+        <v>9026.3671875</v>
       </c>
       <c r="E37" t="n">
-        <v>45.63781324414897</v>
+        <v>81.38665497811712</v>
       </c>
       <c r="F37" t="n">
-        <v>1.212285196900549</v>
+        <v>2.179639449356527</v>
       </c>
       <c r="G37" t="n">
-        <v>0.01228646902941498</v>
+        <v>0.00901654600211965</v>
       </c>
       <c r="H37" t="n">
-        <v>0.0003263676207896842</v>
+        <v>0.0002414747155838022</v>
       </c>
       <c r="I37" t="n">
-        <v>1.054519564228684</v>
+        <v>0.721227100608454</v>
       </c>
       <c r="J37" t="n">
-        <v>0.03664068118368279</v>
+        <v>0.01785733306857111</v>
       </c>
       <c r="K37" t="n">
-        <v>0.0001635296950865214</v>
+        <v>0.0001004126253638873</v>
       </c>
       <c r="L37" t="n">
-        <v>0.03501133786848073</v>
+        <v>0.02</v>
       </c>
       <c r="M37" t="n">
-        <v>130.048828125</v>
+        <v>180.52734375</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -2131,44 +2131,44 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1192.401123046875</v>
+        <v>6837.890625</v>
       </c>
       <c r="E38" t="n">
-        <v>10.17710613310914</v>
+        <v>61.14423462696202</v>
       </c>
       <c r="F38" t="n">
-        <v>0.3490852623853987</v>
+        <v>2.43283311556865</v>
       </c>
       <c r="G38" t="n">
-        <v>0.008534968591025946</v>
+        <v>0.008941973187376337</v>
       </c>
       <c r="H38" t="n">
-        <v>0.0002927582469005068</v>
+        <v>0.000355787076598443</v>
       </c>
       <c r="I38" t="n">
-        <v>0.7448559592145809</v>
+        <v>0.5542966708632717</v>
       </c>
       <c r="J38" t="n">
-        <v>0.03921796391232238</v>
+        <v>0.02302424109636626</v>
       </c>
       <c r="K38" t="n">
-        <v>6.363590322176422e-05</v>
+        <v>0.0001126053621516931</v>
       </c>
       <c r="L38" t="n">
-        <v>0.02800453514739229</v>
+        <v>0.022</v>
       </c>
       <c r="M38" t="n">
-        <v>33.39263916015625</v>
+        <v>150.43359375</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -2176,44 +2176,44 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1566.54052734375</v>
+        <v>7901.3671875</v>
       </c>
       <c r="E39" t="n">
-        <v>13.4757176575362</v>
+        <v>72.61693277193591</v>
       </c>
       <c r="F39" t="n">
-        <v>0.4686037827520356</v>
+        <v>2.621698804344461</v>
       </c>
       <c r="G39" t="n">
-        <v>0.008602214511734234</v>
+        <v>0.009190426295694274</v>
       </c>
       <c r="H39" t="n">
-        <v>0.0002991328820241933</v>
+        <v>0.0003318031857185426</v>
       </c>
       <c r="I39" t="n">
-        <v>0.8801188447743341</v>
+        <v>0.7176820945998618</v>
       </c>
       <c r="J39" t="n">
-        <v>0.04930385523356179</v>
+        <v>0.02887872450328945</v>
       </c>
       <c r="K39" t="n">
-        <v>6.068011308757941e-05</v>
+        <v>0.0001181910140158244</v>
       </c>
       <c r="L39" t="n">
-        <v>0.02600907029478458</v>
+        <v>0.022</v>
       </c>
       <c r="M39" t="n">
-        <v>40.7442626953125</v>
+        <v>173.830078125</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -2221,44 +2221,44 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>3181.53076171875</v>
+        <v>8835.9375</v>
       </c>
       <c r="E40" t="n">
-        <v>35.41241019896221</v>
+        <v>75.33983965195233</v>
       </c>
       <c r="F40" t="n">
-        <v>1.228439457830278</v>
+        <v>2.557140366460105</v>
       </c>
       <c r="G40" t="n">
-        <v>0.01113062008548095</v>
+        <v>0.008526524735145799</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0003861158510900712</v>
+        <v>0.0002894022695905335</v>
       </c>
       <c r="I40" t="n">
-        <v>0.9669665979365619</v>
+        <v>0.7128489007584123</v>
       </c>
       <c r="J40" t="n">
-        <v>0.0371429058873026</v>
+        <v>0.02314669123347024</v>
       </c>
       <c r="K40" t="n">
-        <v>0.0002643694469076908</v>
+        <v>0.0001519252691792823</v>
       </c>
       <c r="L40" t="n">
-        <v>0.02700680272108844</v>
+        <v>0.02</v>
       </c>
       <c r="M40" t="n">
-        <v>85.9229736328125</v>
+        <v>176.71875</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -2266,44 +2266,44 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>3875.9765625</v>
+        <v>9257.8125</v>
       </c>
       <c r="E41" t="n">
-        <v>33.59358828145474</v>
+        <v>89.1534077998639</v>
       </c>
       <c r="F41" t="n">
-        <v>0.6494955415952839</v>
+        <v>3.259690495762425</v>
       </c>
       <c r="G41" t="n">
-        <v>0.008667128848629291</v>
+        <v>0.009630072741251121</v>
       </c>
       <c r="H41" t="n">
-        <v>0.0001675695224473597</v>
+        <v>0.0003521015894156881</v>
       </c>
       <c r="I41" t="n">
-        <v>0.8066232489850158</v>
+        <v>0.3687694104084971</v>
       </c>
       <c r="J41" t="n">
-        <v>0.02168520901320541</v>
+        <v>0.01107179803851206</v>
       </c>
       <c r="K41" t="n">
-        <v>2.732166953704891e-05</v>
+        <v>7.302487491588827e-05</v>
       </c>
       <c r="L41" t="n">
-        <v>0.02498866213151927</v>
+        <v>0.021</v>
       </c>
       <c r="M41" t="n">
-        <v>96.85546875</v>
+        <v>194.4140625</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -2311,44 +2311,44 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>tokay_GG3rearSOAEwf.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1108.9599609375</v>
+        <v>5625.54931640625</v>
       </c>
       <c r="E42" t="n">
-        <v>12.84911246970384</v>
+        <v>51.83701769448351</v>
       </c>
       <c r="F42" t="n">
-        <v>0.4845751917822811</v>
+        <v>2.526739557456056</v>
       </c>
       <c r="G42" t="n">
-        <v>0.01158663335224598</v>
+        <v>0.009214569952005749</v>
       </c>
       <c r="H42" t="n">
-        <v>0.0004369636495916657</v>
+        <v>0.0004491542808250064</v>
       </c>
       <c r="I42" t="n">
-        <v>0.933980869982927</v>
+        <v>0.7835877415703257</v>
       </c>
       <c r="J42" t="n">
-        <v>0.04721403680000062</v>
+        <v>0.04687451605713499</v>
       </c>
       <c r="K42" t="n">
-        <v>0.0002040610114849373</v>
+        <v>0.0002243659335072323</v>
       </c>
       <c r="L42" t="n">
-        <v>0.03199546485260771</v>
+        <v>0.02399092970521542</v>
       </c>
       <c r="M42" t="n">
-        <v>35.481689453125</v>
+        <v>134.962158203125</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -2356,44 +2356,44 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>tokay_GG3rearSOAEwf.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1620.37353515625</v>
+        <v>8096.484375</v>
       </c>
       <c r="E43" t="n">
-        <v>12.01359865548467</v>
+        <v>78.28887462547326</v>
       </c>
       <c r="F43" t="n">
-        <v>0.4437749273019391</v>
+        <v>2.624205836221664</v>
       </c>
       <c r="G43" t="n">
-        <v>0.007414092118164728</v>
+        <v>0.009669489990891665</v>
       </c>
       <c r="H43" t="n">
-        <v>0.0002738719916572487</v>
+        <v>0.0003241167048163005</v>
       </c>
       <c r="I43" t="n">
-        <v>0.8043313981710212</v>
+        <v>0.606666242649432</v>
       </c>
       <c r="J43" t="n">
-        <v>0.04877650692900874</v>
+        <v>0.02019008849351071</v>
       </c>
       <c r="K43" t="n">
-        <v>4.067722807763125e-05</v>
+        <v>0.0001021461108885125</v>
       </c>
       <c r="L43" t="n">
         <v>0.02199546485260771</v>
       </c>
       <c r="M43" t="n">
-        <v>35.640869140625</v>
+        <v>178.0859375</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -2401,44 +2401,44 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>tokay_GG3rearSOAEwf.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>2277.13623046875</v>
+        <v>8489.46533203125</v>
       </c>
       <c r="E44" t="n">
-        <v>19.78648341681066</v>
+        <v>101.9184343584824</v>
       </c>
       <c r="F44" t="n">
-        <v>1.081168630747548</v>
+        <v>3.481792421635467</v>
       </c>
       <c r="G44" t="n">
-        <v>0.008689196171955687</v>
+        <v>0.01200528306228405</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0004747931266830658</v>
+        <v>0.0004101309429344697</v>
       </c>
       <c r="I44" t="n">
-        <v>0.6972401286721835</v>
+        <v>0.941342888221613</v>
       </c>
       <c r="J44" t="n">
-        <v>0.05246166456346101</v>
+        <v>0.03199093798015184</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0001518800121864769</v>
+        <v>0.0003485549518335093</v>
       </c>
       <c r="L44" t="n">
-        <v>0.02399092970521542</v>
+        <v>0.02800453514739229</v>
       </c>
       <c r="M44" t="n">
-        <v>54.630615234375</v>
+        <v>237.7435302734375</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -2446,44 +2446,44 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>tokay_GG3rearSOAEwf.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>3133.0810546875</v>
+        <v>9864.898681640625</v>
       </c>
       <c r="E45" t="n">
-        <v>33.89502375446997</v>
+        <v>92.57374287449112</v>
       </c>
       <c r="F45" t="n">
-        <v>1.263933435150339</v>
+        <v>3.26948592510969</v>
       </c>
       <c r="G45" t="n">
-        <v>0.01081843181291418</v>
+        <v>0.009384155464949513</v>
       </c>
       <c r="H45" t="n">
-        <v>0.0004034154919992666</v>
+        <v>0.0003314262042239185</v>
       </c>
       <c r="I45" t="n">
-        <v>0.899544797048673</v>
+        <v>0.6031090155337008</v>
       </c>
       <c r="J45" t="n">
-        <v>0.03751664806534157</v>
+        <v>0.02156217105194045</v>
       </c>
       <c r="K45" t="n">
-        <v>0.0002401925606323835</v>
+        <v>0.0001095498729547878</v>
       </c>
       <c r="L45" t="n">
-        <v>0.02600907029478458</v>
+        <v>0.02199546485260771</v>
       </c>
       <c r="M45" t="n">
-        <v>81.488525390625</v>
+        <v>216.9830322265625</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -2491,44 +2491,44 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>tokay_GG4rearSOAEwf.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1103.57666015625</v>
+        <v>4944.561767578125</v>
       </c>
       <c r="E46" t="n">
-        <v>12.60328115042385</v>
+        <v>45.28841458447616</v>
       </c>
       <c r="F46" t="n">
-        <v>0.4077147981380755</v>
+        <v>1.798293050157823</v>
       </c>
       <c r="G46" t="n">
-        <v>0.01142039479943279</v>
+        <v>0.009159237302168175</v>
       </c>
       <c r="H46" t="n">
-        <v>0.0003694485511141103</v>
+        <v>0.0003636910882475713</v>
       </c>
       <c r="I46" t="n">
-        <v>1.037320745848272</v>
+        <v>0.5391445149782679</v>
       </c>
       <c r="J46" t="n">
-        <v>0.0454511148003602</v>
+        <v>0.02201095677423928</v>
       </c>
       <c r="K46" t="n">
-        <v>0.0001810533967819043</v>
+        <v>0.0001084582128997591</v>
       </c>
       <c r="L46" t="n">
-        <v>0.03199546485260771</v>
+        <v>0.02199546485260771</v>
       </c>
       <c r="M46" t="n">
-        <v>35.3094482421875</v>
+        <v>108.7579345703125</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -2536,44 +2536,44 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>tokay_GG4rearSOAEwf.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2287.90283203125</v>
+        <v>5768.206787109375</v>
       </c>
       <c r="E47" t="n">
-        <v>22.74092134840308</v>
+        <v>68.8618131122638</v>
       </c>
       <c r="F47" t="n">
-        <v>0.7575725332242673</v>
+        <v>2.105416667748536</v>
       </c>
       <c r="G47" t="n">
-        <v>0.009939635997658694</v>
+        <v>0.01193816651409832</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0003311209386246871</v>
+        <v>0.0003650036736639992</v>
       </c>
       <c r="I47" t="n">
-        <v>0.8623322686978123</v>
+        <v>0.9243709592246925</v>
       </c>
       <c r="J47" t="n">
-        <v>0.03404913086218852</v>
+        <v>0.03284198698865044</v>
       </c>
       <c r="K47" t="n">
-        <v>0.0001603328849093152</v>
+        <v>0.0002025271991541933</v>
       </c>
       <c r="L47" t="n">
-        <v>0.02600907029478458</v>
+        <v>0.03099773242630385</v>
       </c>
       <c r="M47" t="n">
-        <v>59.5062255859375</v>
+        <v>178.8013305664062</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -2581,44 +2581,44 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>tokay_GG4rearSOAEwf.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2845.074462890625</v>
+        <v>7184.014892578125</v>
       </c>
       <c r="E48" t="n">
-        <v>26.00108617660314</v>
+        <v>215.212239384061</v>
       </c>
       <c r="F48" t="n">
-        <v>1.380652296849348</v>
+        <v>3.426336935219513</v>
       </c>
       <c r="G48" t="n">
-        <v>0.009138982657833767</v>
+        <v>0.02995709816893599</v>
       </c>
       <c r="H48" t="n">
-        <v>0.0004852780884499562</v>
+        <v>0.0004769390078463361</v>
       </c>
       <c r="I48" t="n">
-        <v>0.7119528258041408</v>
+        <v>1.272598354498129</v>
       </c>
       <c r="J48" t="n">
-        <v>0.05014480495378063</v>
+        <v>0.01906358170377451</v>
       </c>
       <c r="K48" t="n">
-        <v>0.0001614068421035475</v>
+        <v>0.0004631125362880487</v>
       </c>
       <c r="L48" t="n">
-        <v>0.02399092970521542</v>
+        <v>0.07099773242630386</v>
       </c>
       <c r="M48" t="n">
-        <v>68.2559814453125</v>
+        <v>510.0487670898438</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -2626,38 +2626,38 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>tokay_GG4rearSOAEwf.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>3157.305908203125</v>
+        <v>9633.416748046875</v>
       </c>
       <c r="E49" t="n">
-        <v>30.72764723706822</v>
+        <v>163.3124452650469</v>
       </c>
       <c r="F49" t="n">
-        <v>1.377863286286204</v>
+        <v>3.053847747422519</v>
       </c>
       <c r="G49" t="n">
-        <v>0.009732236321236237</v>
+        <v>0.01695270219656568</v>
       </c>
       <c r="H49" t="n">
-        <v>0.0004364047470681638</v>
+        <v>0.0003170056717458705</v>
       </c>
       <c r="I49" t="n">
-        <v>0.7964899023102103</v>
+        <v>1.103992840979661</v>
       </c>
       <c r="J49" t="n">
-        <v>0.0387277390920288</v>
+        <v>0.01949410344315334</v>
       </c>
       <c r="K49" t="n">
-        <v>0.000257085461072196</v>
+        <v>0.0002697444831906281</v>
       </c>
       <c r="L49" t="n">
-        <v>0.02299319727891156</v>
+        <v>0.04099773242630386</v>
       </c>
       <c r="M49" t="n">
-        <v>72.5965576171875</v>
+        <v>394.9482421875</v>
       </c>
     </row>
     <row r="50">

</xml_diff>